<commit_message>
Refactor timetable generation logic to use a dictionary for daily schedules instead of a list, improving data organization. Update student mapping for H2 and H9, swapping names for accurate representation. Ensure evening and Saturday morning activities are correctly assigned in the timetable.
</commit_message>
<xml_diff>
--- a/student_timetables/Eve LUNG_CampA_timetable.xlsx
+++ b/student_timetables/Eve LUNG_CampA_timetable.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -589,13 +589,14 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>Free Time</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
           <t>Practice 
 (Harp practice room)</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>Private Lesson with Liya HUANG 
+(Room 242)</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -666,20 +667,20 @@
           <t>12:00</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>Private Lesson with Sivan MEGAN 
 (Room 245)</t>
         </is>
       </c>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" s="1" t="n"/>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>Private Lesson with Sivan MEGAN 
-(Room 245)</t>
-        </is>
-      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>Practice 
+(Harp practice room)</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="inlineStr">
         <is>
           <t>Harp MasterClass by Sivan MEGAN 
@@ -825,25 +826,26 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
+          <t>Private Lesson with Gwyneth WENTINK 
+(Room 236)</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
           <t>Practice 
 (Harp practice room)</t>
         </is>
       </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>Free Time</t>
-        </is>
-      </c>
       <c r="D20" s="1" t="inlineStr">
-        <is>
-          <t>Private Lesson with Gwyneth WENTINK 
-(Room 236)</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="inlineStr">
         <is>
           <t>Practice 
 (Harp practice room)</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Private Lesson with Sivan MEGAN 
+(Room 245)</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
@@ -909,32 +911,32 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble 
-(Room 245)</t>
+          <t>Acting Class 
+(Room G13)</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble 
-(Room 245)</t>
+          <t>Acting Class 
+(Room G13)</t>
         </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble 
-(Room 245)</t>
+          <t>Acting Class 
+(Room G13)</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble 
-(Room 245)</t>
+          <t>Acting Class 
+(Room G13)</t>
         </is>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble 
-(Room 245)</t>
+          <t>Group Activity 
+(Room Group Activity)</t>
         </is>
       </c>
       <c r="G24" s="1" t="n"/>
@@ -991,32 +993,31 @@
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Acting Class 
-(Room G13)</t>
+          <t>Ensemble 
+(Room 236)</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>Acting Class 
-(Room G13)</t>
+          <t>Ensemble 
+(Room 236)</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>Acting Class 
-(Room G13)</t>
+          <t>Ensemble 
+(Room 236)</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>Acting Class 
-(Room G13)</t>
+          <t>Ensemble 
+(Room 236)</t>
         </is>
       </c>
       <c r="F28" s="1" t="inlineStr">
         <is>
-          <t>Group Activity 
-(Room Group Activity)</t>
+          <t>Break</t>
         </is>
       </c>
       <c r="G28" s="1" t="n"/>
@@ -1049,28 +1050,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="E7:E14"/>
     <mergeCell ref="E15:E19"/>
     <mergeCell ref="G21:G26"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="B7:B14"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="F24:F27"/>
-    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="F28:F30"/>
     <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D11:D14"/>
     <mergeCell ref="D15:D19"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="F20:F23"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="G7:G14"/>
+    <mergeCell ref="D7:D10"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D7:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C7:C10"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="F15:F19"/>
     <mergeCell ref="D24:D27"/>
@@ -1079,9 +1082,7 @@
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C14"/>
     <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B7:B10"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="B28:B30"/>

</xml_diff>